<commit_message>
migration compte admin reel
</commit_message>
<xml_diff>
--- a/bank/exemples/Tableaux_de_Compte_Administratif.xlsx
+++ b/bank/exemples/Tableaux_de_Compte_Administratif.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="RECETTE"/>
@@ -1962,7 +1962,7 @@
   </sheetPr>
   <dimension ref="A1:N182"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13310,7 +13310,7 @@
   </sheetPr>
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>